<commit_message>
association ternaire - signature - doc xlsx
</commit_message>
<xml_diff>
--- a/test-unitaire-2.xlsx
+++ b/test-unitaire-2.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="0" windowWidth="16680" windowHeight="7620"/>
+    <workbookView xWindow="7560" yWindow="0" windowWidth="16680" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="1" r:id="rId1"/>
-    <sheet name="questions" sheetId="2" r:id="rId2"/>
+    <sheet name="MovieServiceTest" sheetId="4" r:id="rId2"/>
+    <sheet name="questions" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="111">
   <si>
     <t>Intitulé</t>
   </si>
@@ -348,12 +348,315 @@
 Sachant que de manière programmatique, je ne peux modifier l'id d'un bean ()
 L'idée c'est de faire un update (pas un merge programmatique) en passant par une requête ?</t>
   </si>
+  <si>
+    <t>Association 
+@ManyToMany
+caractéristiqe</t>
+  </si>
+  <si>
+    <t>getReference</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>updateActor</t>
+  </si>
+  <si>
+    <t>faire l'update en utilisant movie.addActor</t>
+  </si>
+  <si>
+    <t>Question : je voulais savoir si hibernate détectait que c'était déjà un enregistrement existant</t>
+  </si>
+  <si>
+    <t>ERREUR: la valeur d'une clé dupliquée rompt la contrainte unique « movie_actor_pkey »</t>
+  </si>
+  <si>
+    <t>removeActor</t>
+  </si>
+  <si>
+    <t>Hibernate SQL : 
+select Movie pour mise en session
+select Actor pour mise en session
+Update MovieActor pour mise à jour</t>
+  </si>
+  <si>
+    <t>Modification de l'entité MovieActor</t>
+  </si>
+  <si>
+    <t>addActor_existingMovie()</t>
+  </si>
+  <si>
+    <t>créer un nouvel acteur et l'associer à un film existant</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">IMPORTANT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: il faut faire l'ajout  sur les deux côtés de la relation:</t>
+    </r>
+  </si>
+  <si>
+    <t>Hibernate SQL : 
+insert Actor pour création et mise en session
+select Movie pour mise en session
+Update MovieActor pour mise à jour</t>
+  </si>
+  <si>
+    <t>associateActorAndFilm()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> associe un acteur existant à un film existant</t>
+  </si>
+  <si>
+    <t>Hibernate SQL : 
+select Actor pour mise en session
+select Movie pour mise en session
+Update MovieActor pour mise à jour</t>
+  </si>
+  <si>
+    <t>addMovie_withActor()</t>
+  </si>
+  <si>
+    <t>Service : 
+- créer le film 
+- crer l'acteur 
+- fait l'assocation</t>
+  </si>
+  <si>
+    <t>Service: 
+récupère le film en session
+récupère l'acteur en session
+faire l'association</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Service:
+créer l'acteur pour mise en ession
+' récupère le film en session
+' faire l'association</t>
+  </si>
+  <si>
+    <t>Hibernate SQL : 
+insert Actor pour création et mise en session
+insert Movie pour création et mise en session
+Insert MovieActor en cascade</t>
+  </si>
+  <si>
+    <t>addMovie_existingActor()</t>
+  </si>
+  <si>
+    <t>Service : 
+- créer le film 
+- récupère l'acteur pour mise en session
+- fait l'assocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hibernate SQL : 
+select Acteur pour mise en session
+insert Movie pour création et mise en session
+Insert en cascade MovieActor </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">IMPORTANT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: il faut faire l'ajout  sur les deux côtés de la relation:
+Utilisation de la méthode</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> movie.persist()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+=&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>déclenche en casscade l'insertion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de l'association dans la table Movie_Actor
+A noter : l'insertion peut se faire avec la méthode
+movieService.addMovieActor(Movie, Actor, character)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> créer un nouveau film et associe un acteur existant à ce film
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>movieService.addMovieActorCascade(Movie, Actor, character)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">créer un nouveau film et un nouvel acteur et fait l'association
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>movieService.addMovieActorCascade(Movie, Actor, character)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>movie.UpdateActor(actorBd, movie):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Il suffit juste de mettre à jour le movieActor d'un seul côté de la relation
+- récupère au niveau de movie, le movieActor à modifier
+- impérativement dans la session : Movie, Actor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>movie.removeActor(Actor actor)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">IMPORTANT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: il faut faire la suppression sur les deux côtés de la relation:
+- à partir de Movie
+- à parir de Actor</t>
+    </r>
+  </si>
+  <si>
+    <t>Service : 
+récupère le film en session
+récupère l'acteur en session
+fait la suppression de l'assocation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +693,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -405,7 +724,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -428,11 +747,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -486,6 +842,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -494,17 +859,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -527,6 +910,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -547,6 +940,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -567,6 +970,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -582,6 +995,156 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1041,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,250 +1690,258 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="20" t="s">
+        <v>81</v>
+      </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9" t="s">
+      <c r="G7" s="8"/>
+      <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="8" spans="1:8" ht="39" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="12" t="s">
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D10" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="1:8" ht="39" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="G10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="39" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" ht="39" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-    </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="14"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
     </row>
-    <row r="15" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="39" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
-        <v>3</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="11" t="s">
-        <v>6</v>
+      <c r="A16" s="14"/>
+      <c r="B16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="14"/>
+    <row r="17" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="24">
+        <v>3</v>
+      </c>
+      <c r="B18" s="24"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="14" t="s">
-        <v>8</v>
+      <c r="D18" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
@@ -1378,11 +1949,11 @@
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="4"/>
       <c r="D19" s="14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -1390,29 +1961,23 @@
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="4"/>
       <c r="D20" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>44</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
-        <v>4</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>11</v>
-      </c>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="16" t="s">
-        <v>12</v>
+      <c r="D21" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
@@ -1420,39 +1985,41 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="14"/>
+      <c r="D22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>44</v>
+      </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
-        <v>5</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="7" t="s">
-        <v>15</v>
+      <c r="A23" s="24">
+        <v>4</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="7" t="s">
-        <v>16</v>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -1460,14 +2027,14 @@
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="21">
-        <v>6</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13" t="s">
+      <c r="A25" s="24">
+        <v>5</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="14"/>
@@ -1475,197 +2042,247 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>19</v>
-      </c>
+    <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="24">
+        <v>6</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>17</v>
+      </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>23</v>
-      </c>
+      <c r="D27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="20"/>
+    <row r="28" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="14"/>
+      <c r="D28" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
-      <c r="B29" s="20"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="12"/>
       <c r="D29" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
-      <c r="B30" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="B30" s="23"/>
       <c r="C30" s="12"/>
-      <c r="D30" s="9" t="s">
-        <v>29</v>
+      <c r="D30" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
-      <c r="B31" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="14"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
     </row>
-    <row r="33" spans="1:8" ht="39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
-      <c r="B33" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="11" t="s">
-        <v>33</v>
+      <c r="B33" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
     </row>
+    <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:8" ht="39" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A18:A22"/>
     <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F7">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+  <conditionalFormatting sqref="F8:F9">
+    <cfRule type="cellIs" dxfId="43" priority="25" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="26" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="41" priority="23" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="22" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="37" priority="19" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="20" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="18" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="14" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="todo">
+      <formula>NOT(ISERROR(SEARCH("todo",F4)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="todo">
+      <formula>NOT(ISERROR(SEARCH("todo",F5)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
-      <formula>"ko"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
-      <formula>"ko"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
-      <formula>"ko"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
-      <formula>"ko"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"ko"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"ko"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1675,6 +2292,337 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="33"/>
+      <c r="H5" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="G4:G5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F2:F5">
+    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="todo">
+      <formula>NOT(ISERROR(SEARCH("todo",F2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:F7">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="todo">
+      <formula>NOT(ISERROR(SEARCH("todo",F6)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F16">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="todo">
+      <formula>NOT(ISERROR(SEARCH("todo",F8)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"ko"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C6"/>
   <sheetViews>
@@ -1715,7 +2663,7 @@
       <c r="B6" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
association ternaire  - doc xlsx
</commit_message>
<xml_diff>
--- a/test-unitaire-2.xlsx
+++ b/test-unitaire-2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="0" windowWidth="16680" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="10080" yWindow="0" windowWidth="16680" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
   <si>
     <t>Intitulé</t>
   </si>
@@ -650,6 +650,29 @@
 récupère le film en session
 récupère l'acteur en session
 fait la suppression de l'assocation</t>
+  </si>
+  <si>
+    <t>test qui permet pour un acteur de voir tous ces films</t>
+  </si>
+  <si>
+    <t>test d'ajout d'un acteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- vérifier que le film est supprimé
+- vérifier que les acteurs ne sont pas supprimés
+- vérifier que les assocaitons films-acteurs sont bien supprimés
+</t>
+  </si>
+  <si>
+    <t>test de suppresion d'un film auquels 1 ou plusieurs acteurs sont associés</t>
+  </si>
+  <si>
+    <t>test de suppression d'un acteur auquel 1 ou plusieurs films sont associés</t>
+  </si>
+  <si>
+    <t>- Vérifier que l'acteur est supprimé
+- Vérifier que le ou les films ne sont pas supprimés
+- vérifier que les assocaitons films-acteurs sont bien supprimés</t>
   </si>
 </sst>
 </file>
@@ -850,6 +873,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -865,15 +894,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -882,12 +902,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="33">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1005,116 +1028,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1606,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,10 +1848,10 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="24">
+      <c r="A18" s="26">
         <v>3</v>
       </c>
-      <c r="B18" s="24"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="4"/>
       <c r="D18" s="11" t="s">
         <v>6</v>
@@ -1949,8 +1862,8 @@
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="4"/>
       <c r="D19" s="14" t="s">
         <v>7</v>
@@ -1961,8 +1874,8 @@
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="4"/>
       <c r="D20" s="14" t="s">
         <v>8</v>
@@ -1973,8 +1886,8 @@
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="4"/>
       <c r="D21" s="14" t="s">
         <v>9</v>
@@ -1985,8 +1898,8 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="4"/>
       <c r="D22" s="14" t="s">
         <v>10</v>
@@ -1999,10 +1912,10 @@
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="24">
+      <c r="A23" s="26">
         <v>4</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="4"/>
@@ -2015,8 +1928,8 @@
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="4"/>
       <c r="D24" s="16" t="s">
         <v>13</v>
@@ -2027,10 +1940,10 @@
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="24">
+      <c r="A25" s="26">
         <v>5</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="27" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="17"/>
@@ -2043,8 +1956,8 @@
       <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="17"/>
       <c r="D26" s="7" t="s">
         <v>16</v>
@@ -2055,10 +1968,10 @@
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="24">
+      <c r="A27" s="26">
         <v>6</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="12"/>
@@ -2071,10 +1984,10 @@
       <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="16" t="s">
@@ -2086,7 +1999,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
-      <c r="B29" s="23"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="12"/>
       <c r="D29" s="11" t="s">
         <v>22</v>
@@ -2100,7 +2013,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
-      <c r="B30" s="23"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="12"/>
       <c r="D30" s="11" t="s">
         <v>24</v>
@@ -2112,7 +2025,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
-      <c r="B31" s="23"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="12"/>
       <c r="D31" s="11" t="s">
         <v>25</v>
@@ -2193,96 +2106,96 @@
     <mergeCell ref="A27:A28"/>
   </mergeCells>
   <conditionalFormatting sqref="F8:F9">
-    <cfRule type="cellIs" dxfId="43" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="41" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="23" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="22" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="37" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="18" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="todo">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="todo">
       <formula>NOT(ISERROR(SEARCH("todo",F4)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="todo">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="todo">
       <formula>NOT(ISERROR(SEARCH("todo",F5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2295,7 +2208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -2338,7 +2251,7 @@
       <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>80</v>
       </c>
       <c r="C2" s="19" t="s">
@@ -2362,8 +2275,8 @@
     </row>
     <row r="3" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="24" t="s">
         <v>94</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -2384,8 +2297,8 @@
     </row>
     <row r="4" spans="1:8" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="24" t="s">
         <v>97</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -2397,7 +2310,7 @@
       <c r="F4" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
         <v>105</v>
       </c>
       <c r="H4" s="11" t="s">
@@ -2406,8 +2319,8 @@
     </row>
     <row r="5" spans="1:8" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="24" t="s">
         <v>102</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -2419,15 +2332,15 @@
       <c r="F5" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="33"/>
+      <c r="G5" s="32"/>
       <c r="H5" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="28" t="s">
         <v>83</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -2446,8 +2359,8 @@
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="27"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="9" t="s">
         <v>84</v>
       </c>
@@ -2457,15 +2370,15 @@
       <c r="F7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="33" t="s">
         <v>86</v>
       </c>
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="29" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="23" t="s">
         <v>87</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -2482,11 +2395,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="9"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="E9" s="11"/>
       <c r="F9" s="20" t="s">
         <v>82</v>
@@ -2496,9 +2411,11 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="9" t="s">
+        <v>112</v>
+      </c>
       <c r="E10" s="11"/>
       <c r="F10" s="20" t="s">
         <v>82</v>
@@ -2506,24 +2423,32 @@
       <c r="G10" s="9"/>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="11"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="F11" s="20" t="s">
         <v>82</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="11"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="F12" s="20" t="s">
         <v>82</v>
       </c>
@@ -2532,8 +2457,8 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="9"/>
       <c r="E13" s="11"/>
       <c r="F13" s="20" t="s">
@@ -2544,8 +2469,8 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="9"/>
       <c r="E14" s="11"/>
       <c r="F14" s="20" t="s">
@@ -2556,8 +2481,8 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="9"/>
       <c r="E15" s="11"/>
       <c r="F15" s="20" t="s">
@@ -2581,39 +2506,39 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B2:B8"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="B2:B12"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F5">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="todo">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="todo">
       <formula>NOT(ISERROR(SEARCH("todo",F2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F7">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="todo">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="todo">
       <formula>NOT(ISERROR(SEARCH("todo",F6)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:F16">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="todo">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="todo">
       <formula>NOT(ISERROR(SEARCH("todo",F8)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"ko"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
requetage  - jpql - criteria
</commit_message>
<xml_diff>
--- a/test-unitaire-2.xlsx
+++ b/test-unitaire-2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="0" windowWidth="16680" windowHeight="7620"/>
+    <workbookView xWindow="12225" yWindow="0" windowWidth="16680" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
   <si>
     <t>Intitulé</t>
   </si>
@@ -673,6 +673,20 @@
     <t>- Vérifier que l'acteur est supprimé
 - Vérifier que le ou les films ne sont pas supprimés
 - vérifier que les assocaitons films-acteurs sont bien supprimés</t>
+  </si>
+  <si>
+    <t>getReference_casNominal()</t>
+  </si>
+  <si>
+    <t>remonte un objet proxy</t>
+  </si>
+  <si>
+    <t>'remonte un objet proxy</t>
+  </si>
+  <si>
+    <t>Dans mon cas, dès que le repository fait appel au code
+entityManager.getReference()
+cela déclenche une requêtes Select en base ??</t>
   </si>
 </sst>
 </file>
@@ -879,6 +893,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -894,17 +911,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1519,15 +1533,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -1606,31 +1620,41 @@
       <c r="B4" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="D4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="F4" s="20" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="D5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="F5" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>120</v>
+      </c>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1848,10 +1872,10 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+      <c r="A18" s="27">
         <v>3</v>
       </c>
-      <c r="B18" s="26"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="4"/>
       <c r="D18" s="11" t="s">
         <v>6</v>
@@ -1862,8 +1886,8 @@
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="4"/>
       <c r="D19" s="14" t="s">
         <v>7</v>
@@ -1874,8 +1898,8 @@
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="4"/>
       <c r="D20" s="14" t="s">
         <v>8</v>
@@ -1886,8 +1910,8 @@
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="4"/>
       <c r="D21" s="14" t="s">
         <v>9</v>
@@ -1898,8 +1922,8 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="4"/>
       <c r="D22" s="14" t="s">
         <v>10</v>
@@ -1912,10 +1936,10 @@
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="26">
+      <c r="A23" s="27">
         <v>4</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="4"/>
@@ -1928,8 +1952,8 @@
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="4"/>
       <c r="D24" s="16" t="s">
         <v>13</v>
@@ -1940,10 +1964,10 @@
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="26">
+      <c r="A25" s="27">
         <v>5</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="17"/>
@@ -1956,8 +1980,8 @@
       <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="17"/>
       <c r="D26" s="7" t="s">
         <v>16</v>
@@ -1968,10 +1992,10 @@
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="26">
+      <c r="A27" s="27">
         <v>6</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="12"/>
@@ -1984,8 +2008,8 @@
       <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="12"/>
       <c r="D28" s="7" t="s">
         <v>18</v>
@@ -1999,7 +2023,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
-      <c r="B29" s="25"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="12"/>
       <c r="D29" s="11" t="s">
         <v>22</v>
@@ -2013,7 +2037,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
-      <c r="B30" s="25"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="12"/>
       <c r="D30" s="11" t="s">
         <v>24</v>
@@ -2025,7 +2049,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
-      <c r="B31" s="25"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="12"/>
       <c r="D31" s="11" t="s">
         <v>25</v>
@@ -2251,7 +2275,7 @@
       <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>80</v>
       </c>
       <c r="C2" s="19" t="s">
@@ -2275,7 +2299,7 @@
     </row>
     <row r="3" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="30"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="24" t="s">
         <v>94</v>
       </c>
@@ -2297,7 +2321,7 @@
     </row>
     <row r="4" spans="1:8" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="30"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="24" t="s">
         <v>97</v>
       </c>
@@ -2319,7 +2343,7 @@
     </row>
     <row r="5" spans="1:8" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
-      <c r="B5" s="30"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="24" t="s">
         <v>102</v>
       </c>
@@ -2339,8 +2363,8 @@
     </row>
     <row r="6" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="29" t="s">
         <v>83</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -2359,8 +2383,8 @@
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="9" t="s">
         <v>84</v>
       </c>
@@ -2370,14 +2394,14 @@
       <c r="F7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="25" t="s">
         <v>86</v>
       </c>
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="30"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="23" t="s">
         <v>87</v>
       </c>
@@ -2397,7 +2421,7 @@
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="30"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="23"/>
       <c r="D9" s="9" t="s">
         <v>111</v>
@@ -2411,7 +2435,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="30"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="23"/>
       <c r="D10" s="9" t="s">
         <v>112</v>
@@ -2425,7 +2449,7 @@
     </row>
     <row r="11" spans="1:8" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="30"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="23"/>
       <c r="D11" s="9" t="s">
         <v>114</v>
@@ -2441,7 +2465,7 @@
     </row>
     <row r="12" spans="1:8" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="29"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="23"/>
       <c r="D12" s="9" t="s">
         <v>115</v>

</xml_diff>